<commit_message>
Add Schematic Editor Tile and Clock Gen Pinout
</commit_message>
<xml_diff>
--- a/images/pinout_generation.xlsx
+++ b/images/pinout_generation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdram\Documents\GitHub\gdramos.github.io\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA4D2B0-96C1-400B-8361-E0F27ECCD3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C8FD53-1EA8-4C1B-A1F9-6FDF1DB37BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="12" xr2:uid="{FC8B7902-EF1F-44E2-AC5C-09552D7F3AFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="13" xr2:uid="{FC8B7902-EF1F-44E2-AC5C-09552D7F3AFB}"/>
   </bookViews>
   <sheets>
     <sheet name="74ls00" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,8 @@
     <sheet name="74ls283" sheetId="11" r:id="rId10"/>
     <sheet name="74ls73" sheetId="12" r:id="rId11"/>
     <sheet name="at28c64b" sheetId="14" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId13"/>
+    <sheet name="7-Seg" sheetId="15" r:id="rId13"/>
+    <sheet name="Clk" sheetId="17" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="94">
   <si>
     <t>Vcc</t>
   </si>
@@ -328,6 +329,9 @@
   <si>
     <t>Common Anode 7 Segment Display</t>
   </si>
+  <si>
+    <t>Arduino Clock Generator</t>
+  </si>
 </sst>
 </file>
 
@@ -470,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -517,6 +521,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1861,6 +1868,177 @@
         <a:xfrm>
           <a:off x="6457950" y="676275"/>
           <a:ext cx="4638675" cy="5781675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>59859</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74675E92-1E76-CB0C-4F71-E84E463DB0CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2047875" y="438150"/>
+          <a:ext cx="1762125" cy="4203234"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>274805</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78ADD34E-AF11-DABA-4511-C914CC9D0C12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666750" y="4438650"/>
+          <a:ext cx="4533900" cy="760580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECBE3D6A-1A04-A18C-B27B-5D356DC43C14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6457950" y="371475"/>
+          <a:ext cx="4638675" cy="5181600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7197,7 +7375,7 @@
   <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -7638,8 +7816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6C4868B-8F05-4C53-89C6-EB742AA35EEF}">
   <dimension ref="B1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B2:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -7840,12 +8018,198 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F3D45C-6C4D-4D28-B78F-98756C30EB9B}">
+  <dimension ref="B1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="29.25" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="2:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="20" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B18:H18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4099B64B-C097-474A-9F25-7F54CEC4C505}">
   <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
74LS283 1-index to 0-index pinout
</commit_message>
<xml_diff>
--- a/images/pinout_generation.xlsx
+++ b/images/pinout_generation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gdram\Documents\GitHub\gdramos.github.io\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C8FD53-1EA8-4C1B-A1F9-6FDF1DB37BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB69B6BB-CF4C-4B98-B5A3-D80B334052FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="13" xr2:uid="{FC8B7902-EF1F-44E2-AC5C-09552D7F3AFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="14" xr2:uid="{FC8B7902-EF1F-44E2-AC5C-09552D7F3AFB}"/>
   </bookViews>
   <sheets>
     <sheet name="74ls00" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="at28c64b" sheetId="14" r:id="rId12"/>
     <sheet name="7-Seg" sheetId="15" r:id="rId13"/>
     <sheet name="Clk" sheetId="17" r:id="rId14"/>
+    <sheet name="How to save" sheetId="18" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="99">
   <si>
     <t>Vcc</t>
   </si>
@@ -246,15 +247,6 @@
     <t>S3</t>
   </si>
   <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>B4</t>
-  </si>
-  <si>
-    <t>S4</t>
-  </si>
-  <si>
     <t>Cin</t>
   </si>
   <si>
@@ -331,6 +323,30 @@
   </si>
   <si>
     <t>Arduino Clock Generator</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>S0</t>
+  </si>
+  <si>
+    <t>Select cells to copy</t>
+  </si>
+  <si>
+    <t>See picture</t>
+  </si>
+  <si>
+    <t>Paste</t>
+  </si>
+  <si>
+    <t>Right click</t>
+  </si>
+  <si>
+    <t>Save as picture</t>
   </si>
 </sst>
 </file>
@@ -510,6 +526,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -521,9 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -795,6 +811,67 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="6457950" y="371475"/>
+          <a:ext cx="4991100" cy="5581650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBFB3251-B9EC-B758-7EA8-CC058767EC05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11944350" y="371475"/>
           <a:ext cx="4991100" cy="5581650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1886,6 +1963,67 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A576063-1EB6-5038-F674-8DD9BB039A07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="12553950" y="676275"/>
+          <a:ext cx="4991100" cy="5581650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2053,6 +2191,55 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>237714</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A1C70E5-AC4D-470B-9427-C4387B07B2C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="381000"/>
+          <a:ext cx="3285714" cy="2961905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -6859,7 +7046,7 @@
   <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -7075,15 +7262,15 @@
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="20" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7101,8 +7288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C356852-8636-4621-8846-F40C976D394C}">
   <dimension ref="B1:U24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -7138,12 +7325,12 @@
     <row r="4" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="21" t="s">
         <v>54</v>
       </c>
       <c r="F4" s="12">
@@ -7158,7 +7345,7 @@
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="20"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="12"/>
       <c r="G5" s="14"/>
       <c r="H5" s="15"/>
@@ -7166,17 +7353,17 @@
     <row r="6" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="10"/>
       <c r="C6" s="11" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="12">
         <v>15</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H6" s="15"/>
     </row>
@@ -7184,7 +7371,7 @@
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="20"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="12"/>
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
@@ -7192,17 +7379,17 @@
     <row r="8" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D8" s="12">
         <v>3</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="12">
         <v>14</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="H8" s="15"/>
     </row>
@@ -7210,7 +7397,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="20"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="12"/>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -7218,17 +7405,17 @@
     <row r="10" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="D10" s="12">
         <v>4</v>
       </c>
-      <c r="E10" s="20"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="12">
         <v>13</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="H10" s="15"/>
     </row>
@@ -7236,7 +7423,7 @@
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="20"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="12"/>
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
@@ -7245,17 +7432,17 @@
     <row r="12" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="D12" s="12">
         <v>5</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="12">
         <v>12</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H12" s="15"/>
     </row>
@@ -7263,7 +7450,7 @@
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="12"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
@@ -7271,17 +7458,17 @@
     <row r="14" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="D14" s="12">
         <v>6</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="12">
         <v>11</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H14" s="15"/>
     </row>
@@ -7289,7 +7476,7 @@
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="12"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
@@ -7297,17 +7484,17 @@
     <row r="16" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D16" s="12">
         <v>7</v>
       </c>
-      <c r="E16" s="20"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="12">
         <v>10</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H16" s="15"/>
     </row>
@@ -7315,7 +7502,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="20"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="12"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
@@ -7328,12 +7515,12 @@
       <c r="D18" s="12">
         <v>8</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="12">
         <v>9</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H18" s="15"/>
     </row>
@@ -7347,15 +7534,15 @@
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7411,7 +7598,7 @@
     <row r="4" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D4" s="12">
         <v>1</v>
@@ -7421,7 +7608,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H4" s="15"/>
     </row>
@@ -7459,7 +7646,7 @@
     <row r="8" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D8" s="12">
         <v>3</v>
@@ -7469,7 +7656,7 @@
         <v>12</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H8" s="15"/>
     </row>
@@ -7511,7 +7698,7 @@
     <row r="12" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D12" s="12">
         <v>5</v>
@@ -7521,7 +7708,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H12" s="15"/>
     </row>
@@ -7545,7 +7732,7 @@
         <v>9</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H14" s="15"/>
     </row>
@@ -7561,7 +7748,7 @@
     <row r="16" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D16" s="12">
         <v>7</v>
@@ -7583,15 +7770,15 @@
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="B18" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="20" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7647,7 +7834,7 @@
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
       <c r="D4" s="12"/>
-      <c r="E4" s="20"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="12"/>
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
@@ -7656,7 +7843,7 @@
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="20"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="12"/>
       <c r="G5" s="14"/>
       <c r="H5" s="15"/>
@@ -7665,7 +7852,7 @@
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
-      <c r="E6" s="20"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="12"/>
       <c r="G6" s="14"/>
       <c r="H6" s="15"/>
@@ -7674,7 +7861,7 @@
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="20"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="12"/>
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
@@ -7683,7 +7870,7 @@
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="20"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="12"/>
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
@@ -7692,7 +7879,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="20"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="12"/>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -7701,7 +7888,7 @@
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="20"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="12"/>
       <c r="G10" s="14"/>
       <c r="H10" s="15"/>
@@ -7710,7 +7897,7 @@
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="20"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="12"/>
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
@@ -7720,7 +7907,7 @@
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="12"/>
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
@@ -7729,7 +7916,7 @@
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="12"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
@@ -7738,7 +7925,7 @@
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="20"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="12"/>
       <c r="G14" s="14"/>
       <c r="H14" s="15"/>
@@ -7747,7 +7934,7 @@
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="12"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
@@ -7756,7 +7943,7 @@
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="20"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="12"/>
       <c r="G16" s="14"/>
       <c r="H16" s="15"/>
@@ -7765,7 +7952,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="20"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="12"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
@@ -7774,7 +7961,7 @@
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="12"/>
       <c r="G18" s="14"/>
       <c r="H18" s="15"/>
@@ -7789,15 +7976,15 @@
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="B20" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7817,7 +8004,7 @@
   <dimension ref="B1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B2:H20"/>
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.45"/>
@@ -7854,7 +8041,7 @@
       <c r="B4" s="10"/>
       <c r="C4" s="11"/>
       <c r="D4" s="12"/>
-      <c r="E4" s="20"/>
+      <c r="E4" s="21"/>
       <c r="F4" s="12"/>
       <c r="G4" s="14"/>
       <c r="H4" s="15"/>
@@ -7863,7 +8050,7 @@
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="20"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="12"/>
       <c r="G5" s="14"/>
       <c r="H5" s="15"/>
@@ -7872,7 +8059,7 @@
       <c r="B6" s="10"/>
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
-      <c r="E6" s="20"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="12"/>
       <c r="G6" s="14"/>
       <c r="H6" s="15"/>
@@ -7881,7 +8068,7 @@
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="20"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="12"/>
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
@@ -7890,7 +8077,7 @@
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="20"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="12"/>
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
@@ -7899,7 +8086,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="20"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="12"/>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -7908,7 +8095,7 @@
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="20"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="12"/>
       <c r="G10" s="14"/>
       <c r="H10" s="15"/>
@@ -7917,7 +8104,7 @@
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="20"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="12"/>
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
@@ -7927,7 +8114,7 @@
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
       <c r="D12" s="12"/>
-      <c r="E12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="12"/>
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
@@ -7936,7 +8123,7 @@
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="12"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
@@ -7945,7 +8132,7 @@
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="20"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="12"/>
       <c r="G14" s="14"/>
       <c r="H14" s="15"/>
@@ -7954,7 +8141,7 @@
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="12"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
@@ -7963,7 +8150,7 @@
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="20"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="12"/>
       <c r="G16" s="14"/>
       <c r="H16" s="15"/>
@@ -7972,7 +8159,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="20"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="12"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
@@ -7981,7 +8168,7 @@
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="12"/>
       <c r="G18" s="14"/>
       <c r="H18" s="15"/>
@@ -7996,15 +8183,15 @@
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="B20" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8014,7 +8201,8 @@
     <mergeCell ref="B20:H20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8022,7 +8210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F3D45C-6C4D-4D28-B78F-98756C30EB9B}">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
@@ -8168,7 +8356,7 @@
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="12"/>
-      <c r="E16" s="21"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="12"/>
       <c r="G16" s="14"/>
       <c r="H16" s="15"/>
@@ -8183,15 +8371,15 @@
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="B18" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="20" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8199,6 +8387,62 @@
   <mergeCells count="1">
     <mergeCell ref="B18:H18"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1C7CA9-F17C-494F-ABE1-06F0F2925A8D}">
+  <dimension ref="A2:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -8425,15 +8669,15 @@
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="20" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8668,15 +8912,15 @@
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="20" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8911,15 +9155,15 @@
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="20" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8977,7 +9221,7 @@
       <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="21" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="12">
@@ -8992,7 +9236,7 @@
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="20"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="12"/>
       <c r="G5" s="14"/>
       <c r="H5" s="15"/>
@@ -9003,7 +9247,7 @@
       <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="12">
         <v>15</v>
       </c>
@@ -9016,7 +9260,7 @@
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="20"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="12"/>
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
@@ -9027,7 +9271,7 @@
       <c r="D8" s="12">
         <v>3</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="12">
         <v>14</v>
       </c>
@@ -9040,7 +9284,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="20"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="12"/>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -9051,7 +9295,7 @@
       <c r="D10" s="12">
         <v>4</v>
       </c>
-      <c r="E10" s="20"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="12">
         <v>13</v>
       </c>
@@ -9064,7 +9308,7 @@
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="20"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="12"/>
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
@@ -9076,7 +9320,7 @@
       <c r="D12" s="12">
         <v>5</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="12">
         <v>12</v>
       </c>
@@ -9089,7 +9333,7 @@
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="12"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
@@ -9100,7 +9344,7 @@
       <c r="D14" s="12">
         <v>6</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="12">
         <v>11</v>
       </c>
@@ -9113,7 +9357,7 @@
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="12"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
@@ -9124,7 +9368,7 @@
       <c r="D16" s="12">
         <v>7</v>
       </c>
-      <c r="E16" s="20"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="12">
         <v>10</v>
       </c>
@@ -9137,7 +9381,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="20"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="12"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
@@ -9150,7 +9394,7 @@
       <c r="D18" s="12">
         <v>8</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="12">
         <v>9</v>
       </c>
@@ -9169,15 +9413,15 @@
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -9413,15 +9657,15 @@
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="20" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -9479,7 +9723,7 @@
       <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="21" t="s">
         <v>40</v>
       </c>
       <c r="F4" s="12">
@@ -9494,7 +9738,7 @@
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="20"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="12"/>
       <c r="G5" s="14"/>
       <c r="H5" s="15"/>
@@ -9505,7 +9749,7 @@
       <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="12">
         <v>15</v>
       </c>
@@ -9518,7 +9762,7 @@
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="20"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="12"/>
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
@@ -9529,7 +9773,7 @@
       <c r="D8" s="12">
         <v>3</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="12">
         <v>14</v>
       </c>
@@ -9542,7 +9786,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="20"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="12"/>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -9553,7 +9797,7 @@
       <c r="D10" s="12">
         <v>4</v>
       </c>
-      <c r="E10" s="20"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="12">
         <v>13</v>
       </c>
@@ -9566,7 +9810,7 @@
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="20"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="12"/>
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
@@ -9578,7 +9822,7 @@
       <c r="D12" s="12">
         <v>5</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="12">
         <v>12</v>
       </c>
@@ -9591,7 +9835,7 @@
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="12"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
@@ -9599,12 +9843,12 @@
     <row r="14" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D14" s="12">
         <v>6</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="12">
         <v>11</v>
       </c>
@@ -9617,7 +9861,7 @@
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="12"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
@@ -9630,7 +9874,7 @@
       <c r="D16" s="12">
         <v>7</v>
       </c>
-      <c r="E16" s="20"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="12">
         <v>10</v>
       </c>
@@ -9643,7 +9887,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="20"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="12"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
@@ -9656,7 +9900,7 @@
       <c r="D18" s="12">
         <v>8</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="12">
         <v>9</v>
       </c>
@@ -9675,15 +9919,15 @@
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -9744,7 +9988,7 @@
       <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="21" t="s">
         <v>42</v>
       </c>
       <c r="F4" s="12">
@@ -9759,7 +10003,7 @@
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="20"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="12"/>
       <c r="G5" s="14"/>
       <c r="H5" s="15"/>
@@ -9772,7 +10016,7 @@
       <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="12">
         <v>15</v>
       </c>
@@ -9785,7 +10029,7 @@
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="20"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="12"/>
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
@@ -9798,7 +10042,7 @@
       <c r="D8" s="12">
         <v>3</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="12">
         <v>14</v>
       </c>
@@ -9811,7 +10055,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="20"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="12"/>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -9824,7 +10068,7 @@
       <c r="D10" s="12">
         <v>4</v>
       </c>
-      <c r="E10" s="20"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="12">
         <v>13</v>
       </c>
@@ -9837,7 +10081,7 @@
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="20"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="12"/>
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
@@ -9846,12 +10090,12 @@
     <row r="12" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D12" s="12">
         <v>5</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="12">
         <v>12</v>
       </c>
@@ -9864,7 +10108,7 @@
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="12"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
@@ -9875,7 +10119,7 @@
       <c r="D14" s="12">
         <v>6</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="12">
         <v>11</v>
       </c>
@@ -9886,7 +10130,7 @@
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="12"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
@@ -9897,7 +10141,7 @@
       <c r="D16" s="12">
         <v>7</v>
       </c>
-      <c r="E16" s="20"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="12">
         <v>10</v>
       </c>
@@ -9908,7 +10152,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="20"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="12"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
@@ -9921,7 +10165,7 @@
       <c r="D18" s="12">
         <v>8</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="12">
         <v>9</v>
       </c>
@@ -9938,15 +10182,15 @@
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -10005,7 +10249,7 @@
       <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="21" t="s">
         <v>52</v>
       </c>
       <c r="F4" s="12">
@@ -10020,7 +10264,7 @@
       <c r="B5" s="10"/>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
-      <c r="E5" s="20"/>
+      <c r="E5" s="21"/>
       <c r="F5" s="12"/>
       <c r="G5" s="14"/>
       <c r="H5" s="15"/>
@@ -10031,7 +10275,7 @@
       <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="21"/>
       <c r="F6" s="12">
         <v>15</v>
       </c>
@@ -10042,7 +10286,7 @@
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="20"/>
+      <c r="E7" s="21"/>
       <c r="F7" s="12"/>
       <c r="G7" s="14"/>
       <c r="H7" s="15"/>
@@ -10050,12 +10294,12 @@
     <row r="8" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="10"/>
       <c r="C8" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D8" s="12">
         <v>3</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="12">
         <v>14</v>
       </c>
@@ -10066,7 +10310,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
-      <c r="E9" s="20"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="12"/>
       <c r="G9" s="14"/>
       <c r="H9" s="15"/>
@@ -10074,17 +10318,17 @@
     <row r="10" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="10"/>
       <c r="C10" s="11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D10" s="12">
         <v>4</v>
       </c>
-      <c r="E10" s="20"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="12">
         <v>13</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H10" s="15"/>
     </row>
@@ -10092,7 +10336,7 @@
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="20"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="12"/>
       <c r="G11" s="14"/>
       <c r="H11" s="15"/>
@@ -10101,17 +10345,17 @@
     <row r="12" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D12" s="12">
         <v>5</v>
       </c>
-      <c r="E12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="12">
         <v>12</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H12" s="15"/>
     </row>
@@ -10119,7 +10363,7 @@
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
-      <c r="E13" s="20"/>
+      <c r="E13" s="21"/>
       <c r="F13" s="12"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
@@ -10127,17 +10371,17 @@
     <row r="14" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D14" s="12">
         <v>6</v>
       </c>
-      <c r="E14" s="20"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="12">
         <v>11</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H14" s="15"/>
     </row>
@@ -10145,7 +10389,7 @@
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
       <c r="F15" s="12"/>
       <c r="G15" s="14"/>
       <c r="H15" s="15"/>
@@ -10153,17 +10397,17 @@
     <row r="16" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D16" s="12">
         <v>7</v>
       </c>
-      <c r="E16" s="20"/>
+      <c r="E16" s="21"/>
       <c r="F16" s="12">
         <v>10</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H16" s="15"/>
     </row>
@@ -10171,7 +10415,7 @@
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="20"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="12"/>
       <c r="G17" s="14"/>
       <c r="H17" s="15"/>
@@ -10184,12 +10428,12 @@
       <c r="D18" s="12">
         <v>8</v>
       </c>
-      <c r="E18" s="20"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="12">
         <v>9</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H18" s="15"/>
     </row>
@@ -10203,15 +10447,15 @@
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="2:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="22" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>